<commit_message>
ran with more recent gps data
</commit_message>
<xml_diff>
--- a/output/Delivered to Xin 2024.xlsx
+++ b/output/Delivered to Xin 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansleybr\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD5D36B-C178-4EA4-B472-7081C6B39DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5411DC5E-CBCB-4578-B950-8CC409F4D090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>name</t>
   </si>
@@ -88,6 +88,42 @@
   </si>
   <si>
     <t>Date Delivered to Xin</t>
+  </si>
+  <si>
+    <t>PT18-8JL</t>
+  </si>
+  <si>
+    <t>63fe40d54e373f000e48fc33</t>
+  </si>
+  <si>
+    <t>6444912fc88148000f6fa7de</t>
+  </si>
+  <si>
+    <t>6442e43fc88148000dd996d8</t>
+  </si>
+  <si>
+    <t>6442e440c88148000dd996d9</t>
+  </si>
+  <si>
+    <t>WS8-E6A</t>
+  </si>
+  <si>
+    <t>65c153d5a5f597000d44a13f</t>
+  </si>
+  <si>
+    <t>65c153d5eeacfe000de00969</t>
+  </si>
+  <si>
+    <t>65c297d613a987000d2e1e50</t>
+  </si>
+  <si>
+    <t>65c297d713a987000d2e1e51</t>
+  </si>
+  <si>
+    <t>WS16-97M</t>
+  </si>
+  <si>
+    <t>PT14-8BY</t>
   </si>
 </sst>
 </file>
@@ -123,9 +159,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,15 +443,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -454,7 +499,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -474,7 +519,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -494,7 +539,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -514,7 +559,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -533,6 +578,89 @@
       <c r="F6" s="1">
         <v>45447</v>
       </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>45.498005999999997</v>
+      </c>
+      <c r="E8">
+        <v>-107.696585</v>
+      </c>
+      <c r="F8" s="1">
+        <v>45449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>45.697949000000001</v>
+      </c>
+      <c r="E9">
+        <v>-107.63875400000001</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45449</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>45.898358000000002</v>
+      </c>
+      <c r="E10">
+        <v>-107.58851799999999</v>
+      </c>
+      <c r="F10" s="1">
+        <v>45449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>45.816850000000002</v>
+      </c>
+      <c r="E11">
+        <v>-107.621486</v>
+      </c>
+      <c r="F11" s="1">
+        <v>45449</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated with deployed sensors 25 Jun 24
</commit_message>
<xml_diff>
--- a/output/Delivered to Xin 2024.xlsx
+++ b/output/Delivered to Xin 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansleybr\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5411DC5E-CBCB-4578-B950-8CC409F4D090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA905D82-AE66-4073-BCB8-BA779B768585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -124,6 +124,42 @@
   </si>
   <si>
     <t>PT14-8BY</t>
+  </si>
+  <si>
+    <t>PT11-SPF</t>
+  </si>
+  <si>
+    <t>6444fa9dbca6e305b2e2c466</t>
+  </si>
+  <si>
+    <t>6444fa9e4426821a1c8b91a9</t>
+  </si>
+  <si>
+    <t>WS34-YKL</t>
+  </si>
+  <si>
+    <t>6601c717158679306b7ee056</t>
+  </si>
+  <si>
+    <t>6601c717f7bd28322857b8bb</t>
+  </si>
+  <si>
+    <t>WS35-F4R</t>
+  </si>
+  <si>
+    <t>6601c966ca0eeb3251d33804</t>
+  </si>
+  <si>
+    <t>6601c9664bbb713194d31a6a</t>
+  </si>
+  <si>
+    <t>WS36-DK3</t>
+  </si>
+  <si>
+    <t>6601cbf05fe5e133cd1dd980</t>
+  </si>
+  <si>
+    <t>6601cbf1022d5e321084e51a</t>
   </si>
 </sst>
 </file>
@@ -443,23 +479,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -499,7 +535,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -519,7 +555,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -539,7 +575,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -559,7 +595,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -579,7 +615,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -599,7 +635,7 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -619,7 +655,7 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -639,7 +675,7 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -659,8 +695,88 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>45.349024</v>
+      </c>
+      <c r="E13">
+        <v>-108.89264900000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>45468</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>45.660300999999997</v>
+      </c>
+      <c r="E14">
+        <v>-108.850004</v>
+      </c>
+      <c r="F14" s="1">
+        <v>45468</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15">
+        <v>45.431862000000002</v>
+      </c>
+      <c r="E15">
+        <v>-108.882907</v>
+      </c>
+      <c r="F15" s="1">
+        <v>45468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16">
+        <v>45.502678000000003</v>
+      </c>
+      <c r="E16">
+        <v>-108.861688</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45468</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated GPS points for Leah Wimmer
</commit_message>
<xml_diff>
--- a/output/Delivered to Xin 2024.xlsx
+++ b/output/Delivered to Xin 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansleybr\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA905D82-AE66-4073-BCB8-BA779B768585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0085BE-3EC8-4375-8C50-F5D894FBCA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
@@ -160,6 +160,33 @@
   </si>
   <si>
     <t>6601cbf1022d5e321084e51a</t>
+  </si>
+  <si>
+    <t>PT23-3SW</t>
+  </si>
+  <si>
+    <t>6667296e59252dd20e4b0624</t>
+  </si>
+  <si>
+    <t>6667296ee1a5e4d5981aa69a</t>
+  </si>
+  <si>
+    <t>WS15-NUJ</t>
+  </si>
+  <si>
+    <t>65c295c692b375000a504151</t>
+  </si>
+  <si>
+    <t>65c295c639f940000d986a2e</t>
+  </si>
+  <si>
+    <t>WS38-G4T</t>
+  </si>
+  <si>
+    <t>6601cf2a42c3f332558616a5</t>
+  </si>
+  <si>
+    <t>6601cf2a2099c433035b02b1</t>
   </si>
 </sst>
 </file>
@@ -479,23 +506,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -535,7 +562,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -555,7 +582,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -575,7 +602,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -595,7 +622,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -615,7 +642,7 @@
         <v>45447</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -635,7 +662,7 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -655,7 +682,7 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -675,7 +702,7 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -695,10 +722,10 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -718,7 +745,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -738,7 +765,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -758,7 +785,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -776,6 +803,66 @@
       </c>
       <c r="F16" s="1">
         <v>45468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>44.742688000000001</v>
+      </c>
+      <c r="E18">
+        <v>-108.910799</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>44.837573999999996</v>
+      </c>
+      <c r="E19">
+        <v>-108.404335</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20">
+        <v>44.837573999999996</v>
+      </c>
+      <c r="E20">
+        <v>-108.404335</v>
+      </c>
+      <c r="F20" s="1">
+        <v>45469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
launched Kreg and Mark sensors
</commit_message>
<xml_diff>
--- a/output/Delivered to Xin 2024.xlsx
+++ b/output/Delivered to Xin 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansleybr\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0085BE-3EC8-4375-8C50-F5D894FBCA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55365D0-84A1-4A6D-BFA8-082A2265222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="5400" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>name</t>
   </si>
@@ -187,6 +187,78 @@
   </si>
   <si>
     <t>6601cf2a2099c433035b02b1</t>
+  </si>
+  <si>
+    <t>PT9-M8U</t>
+  </si>
+  <si>
+    <t>645156ce47e3b51c2399761a</t>
+  </si>
+  <si>
+    <t>645156cf1ca5eb000db782ae</t>
+  </si>
+  <si>
+    <t>WS7-7R8</t>
+  </si>
+  <si>
+    <t>65c14dc29deec5000eb8c4ec</t>
+  </si>
+  <si>
+    <t>65c14dc29deec5000c8f3edc</t>
+  </si>
+  <si>
+    <t>WS47-6P9</t>
+  </si>
+  <si>
+    <t>6644d5387d2393000b8b9e7f</t>
+  </si>
+  <si>
+    <t>6644d5387d2393000b8b9e80</t>
+  </si>
+  <si>
+    <t>PT16-VMF</t>
+  </si>
+  <si>
+    <t>6446abe57e1943000ed84f1a</t>
+  </si>
+  <si>
+    <t>6446abe5d4c889000e636142</t>
+  </si>
+  <si>
+    <t>WS5-G2N</t>
+  </si>
+  <si>
+    <t>65c13e5463c11f000d32382c</t>
+  </si>
+  <si>
+    <t>65c13e559deec5000eb8c4ea</t>
+  </si>
+  <si>
+    <t>WS3-NYM</t>
+  </si>
+  <si>
+    <t>65c13224b78889000c09cfb4</t>
+  </si>
+  <si>
+    <t>65c1322429e691000e783bc4</t>
+  </si>
+  <si>
+    <t>Mark Bjornstead</t>
+  </si>
+  <si>
+    <t>Kreg Vollmer</t>
+  </si>
+  <si>
+    <t>Leah Wimmer</t>
+  </si>
+  <si>
+    <t>Stephen Rose</t>
+  </si>
+  <si>
+    <t>Alyssa Brewer</t>
+  </si>
+  <si>
+    <t>Andy Stieger</t>
   </si>
 </sst>
 </file>
@@ -506,23 +578,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -561,8 +633,11 @@
       <c r="F2" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -581,8 +656,11 @@
       <c r="F3" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -601,8 +679,11 @@
       <c r="F4" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -621,8 +702,11 @@
       <c r="F5" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -641,8 +725,11 @@
       <c r="F6" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -661,8 +748,11 @@
       <c r="F8" s="1">
         <v>45449</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -681,8 +771,11 @@
       <c r="F9" s="1">
         <v>45449</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -701,8 +794,11 @@
       <c r="F10" s="1">
         <v>45449</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -721,11 +817,14 @@
       <c r="F11" s="1">
         <v>45449</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -744,8 +843,11 @@
       <c r="F13" s="1">
         <v>45468</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -764,8 +866,11 @@
       <c r="F14" s="1">
         <v>45468</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -784,8 +889,11 @@
       <c r="F15" s="1">
         <v>45468</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -804,8 +912,11 @@
       <c r="F16" s="1">
         <v>45468</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -824,8 +935,11 @@
       <c r="F18" s="1">
         <v>45469</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -844,8 +958,11 @@
       <c r="F19" s="1">
         <v>45469</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -863,6 +980,147 @@
       </c>
       <c r="F20" s="1">
         <v>45469</v>
+      </c>
+      <c r="G20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22">
+        <v>44.205145999999999</v>
+      </c>
+      <c r="E22">
+        <v>-107.92413500000001</v>
+      </c>
+      <c r="F22" s="1">
+        <v>45470</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23">
+        <v>40.542369999999998</v>
+      </c>
+      <c r="E23">
+        <v>-102.2972</v>
+      </c>
+      <c r="F23" s="1">
+        <v>45470</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24">
+        <v>41.062220000000003</v>
+      </c>
+      <c r="E24">
+        <v>-101.95968999999999</v>
+      </c>
+      <c r="F24" s="1">
+        <v>45470</v>
+      </c>
+      <c r="G24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25">
+        <v>40.774619999999999</v>
+      </c>
+      <c r="E25">
+        <v>-103.03641</v>
+      </c>
+      <c r="F25" s="1">
+        <v>45470</v>
+      </c>
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26">
+        <v>41.105719999999998</v>
+      </c>
+      <c r="E26">
+        <v>-101.69614</v>
+      </c>
+      <c r="F26" s="1">
+        <v>45470</v>
+      </c>
+      <c r="G26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27">
+        <v>40.581780000000002</v>
+      </c>
+      <c r="E27">
+        <v>-102.03254</v>
+      </c>
+      <c r="F27" s="1">
+        <v>45470</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added exe file for easy use
</commit_message>
<xml_diff>
--- a/output/Delivered to Xin 2024.xlsx
+++ b/output/Delivered to Xin 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55365D0-84A1-4A6D-BFA8-082A2265222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1625ADA9-3829-44A5-B98A-B5E4BCD3A20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="5400" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
   <si>
     <t>name</t>
   </si>
@@ -259,6 +259,84 @@
   </si>
   <si>
     <t>Andy Stieger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stewart Norrish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stewart  Norrish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ella Stankiewicz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark Bjornestad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ella </t>
+  </si>
+  <si>
+    <t>WS17-WLE</t>
+  </si>
+  <si>
+    <t>PT7-VD9</t>
+  </si>
+  <si>
+    <t>WS48-ABS</t>
+  </si>
+  <si>
+    <t>WS27-XLU</t>
+  </si>
+  <si>
+    <t>WS10-C67</t>
+  </si>
+  <si>
+    <t>65c29a0b39f940000d986a32</t>
+  </si>
+  <si>
+    <t>65c29a0ba6f677000ddd0937</t>
+  </si>
+  <si>
+    <t>667dd9e00cb3d2000e8458f0</t>
+  </si>
+  <si>
+    <t>667dd9e0dea5cc000edfc671</t>
+  </si>
+  <si>
+    <t>648b4aa004a601000d19a6f7</t>
+  </si>
+  <si>
+    <t>648b4aa166b6ec000ff468ec</t>
+  </si>
+  <si>
+    <t>6644f0dd573ffb000ce2b97f</t>
+  </si>
+  <si>
+    <t>6644f0ddb921b4000b90b85d</t>
+  </si>
+  <si>
+    <t>65d6457c7a715d000bf94dc0</t>
+  </si>
+  <si>
+    <t>65d6457d7a715d000c7d068c</t>
+  </si>
+  <si>
+    <t>WS37-4NE</t>
+  </si>
+  <si>
+    <t>6601cdd45f4c803643ea5668</t>
+  </si>
+  <si>
+    <t>6601cdd45fe5e134ed5d28be</t>
+  </si>
+  <si>
+    <t>WS12-ESF</t>
+  </si>
+  <si>
+    <t>6633cda1efd480018020fc75</t>
+  </si>
+  <si>
+    <t>6633cda2972270000bb4ffca</t>
   </si>
 </sst>
 </file>
@@ -578,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1123,6 +1201,167 @@
         <v>73</v>
       </c>
     </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29">
+        <v>40.316295459999999</v>
+      </c>
+      <c r="E29">
+        <v>-103.5642296</v>
+      </c>
+      <c r="F29" s="1">
+        <v>45474</v>
+      </c>
+      <c r="G29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30">
+        <v>44.695286350000003</v>
+      </c>
+      <c r="E30">
+        <v>-108.7679644</v>
+      </c>
+      <c r="F30" s="1">
+        <v>45474</v>
+      </c>
+      <c r="G30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31">
+        <v>40.144148600000001</v>
+      </c>
+      <c r="E31">
+        <v>-102.6879031</v>
+      </c>
+      <c r="F31" s="1">
+        <v>45474</v>
+      </c>
+      <c r="G31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32">
+        <v>40.290162100000003</v>
+      </c>
+      <c r="E32">
+        <v>-104.8992951</v>
+      </c>
+      <c r="F32" s="1">
+        <v>45474</v>
+      </c>
+      <c r="G32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33">
+        <v>39.962213920000003</v>
+      </c>
+      <c r="E33">
+        <v>-102.29797979999999</v>
+      </c>
+      <c r="F33" s="1">
+        <v>45474</v>
+      </c>
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>44.5044781</v>
+      </c>
+      <c r="E34">
+        <v>-108.3984542</v>
+      </c>
+      <c r="F34" s="1">
+        <v>45474</v>
+      </c>
+      <c r="G34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35">
+        <v>40.135103569999998</v>
+      </c>
+      <c r="E35">
+        <v>-105.0301903</v>
+      </c>
+      <c r="F35" s="1">
+        <v>45474</v>
+      </c>
+      <c r="G35" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated with new sensor launch
</commit_message>
<xml_diff>
--- a/output/Delivered to Xin 2024.xlsx
+++ b/output/Delivered to Xin 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1625ADA9-3829-44A5-B98A-B5E4BCD3A20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DA6130-5937-498A-AA95-F2F0CDEC3E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="5400" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
@@ -337,6 +337,30 @@
   </si>
   <si>
     <t>6633cda2972270000bb4ffca</t>
+  </si>
+  <si>
+    <t>WS20-CXA</t>
+  </si>
+  <si>
+    <t>65c3c5102e3cdb000d09150d</t>
+  </si>
+  <si>
+    <t>65c3c51148bb6b000d333ba5</t>
+  </si>
+  <si>
+    <t>PT15-6A5</t>
+  </si>
+  <si>
+    <t>63fd2c8f4b3d79000b91720d</t>
+  </si>
+  <si>
+    <t>6440333064e2e2000d87d60d</t>
+  </si>
+  <si>
+    <t>Terry Weber</t>
+  </si>
+  <si>
+    <t>Stewart Norrish</t>
   </si>
 </sst>
 </file>
@@ -656,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:E28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1362,6 +1386,75 @@
         <v>82</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37">
+        <v>40.307834999999997</v>
+      </c>
+      <c r="E37">
+        <v>-104.777721</v>
+      </c>
+      <c r="F37" s="1">
+        <v>45482</v>
+      </c>
+      <c r="G37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38">
+        <v>39.962213920000003</v>
+      </c>
+      <c r="E38">
+        <v>-102.29797979999999</v>
+      </c>
+      <c r="F38" s="1">
+        <v>45482</v>
+      </c>
+      <c r="G38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39">
+        <v>40.498097999999999</v>
+      </c>
+      <c r="E39">
+        <v>-104.59709599999999</v>
+      </c>
+      <c r="F39" s="1">
+        <v>45482</v>
+      </c>
+      <c r="G39" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Delivered to Xin 2024.xlsx
</commit_message>
<xml_diff>
--- a/output/Delivered to Xin 2024.xlsx
+++ b/output/Delivered to Xin 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colostate.sharepoint.com/sites/AWQP_Sharepoint/Shared Documents/Water_Quality_Project/Research/PileTemp_Cercospora Systems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B349D7EF-3FE4-42E7-962E-9FB19B3E507C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="384" documentId="13_ncr:1_{A6DA6130-5937-498A-AA95-F2F0CDEC3E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{975090C0-EC95-4706-922E-B4DC02CEC9EA}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="5400" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="177">
   <si>
     <t>name</t>
   </si>
@@ -86,6 +86,9 @@
     <t>Status (12 July)</t>
   </si>
   <si>
+    <t>Status (15 July)</t>
+  </si>
+  <si>
     <t>Notes on 2023 (if deployed)</t>
   </si>
   <si>
@@ -158,6 +161,9 @@
     <t>Bad*</t>
   </si>
   <si>
+    <t>Bad (Bad Data)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Good for the most part, Ends with bad but give infection rate </t>
   </si>
   <si>
@@ -245,6 +251,9 @@
     <t>6601c717f7bd28322857b8bb</t>
   </si>
   <si>
+    <t>Bad (Dead battery; Bad Data)</t>
+  </si>
+  <si>
     <t>WS35-F4R</t>
   </si>
   <si>
@@ -395,6 +404,9 @@
     <t>65c13e559deec5000eb8c4ea</t>
   </si>
   <si>
+    <t>Bad* Dead Battery, However, Green on dashboard, but most recent shows bad data for 2 days</t>
+  </si>
+  <si>
     <t>Bad till 7/10, now good</t>
   </si>
   <si>
@@ -488,6 +500,9 @@
     <t>65d6457d7a715d000c7d068c</t>
   </si>
   <si>
+    <t>Bad (just got new battery, so wait 2 days?)</t>
+  </si>
+  <si>
     <t>WS37-4NE</t>
   </si>
   <si>
@@ -530,6 +545,9 @@
     <t>Stewart Norrish</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>Good since deployment 7/1; Stewart submitted survey123 twice; this is duplicate of row 33</t>
   </si>
   <si>
@@ -564,6 +582,12 @@
   </si>
   <si>
     <t>What's the difference between "Bad" and "Missing" Data?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal Drops around 3am </t>
+  </si>
+  <si>
+    <t>WS5 showing up as green on dashboard but shows "bad data" for last two days (note on 7/15)</t>
   </si>
 </sst>
 </file>
@@ -579,7 +603,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -589,6 +613,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -619,10 +649,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -652,10 +692,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>572877</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>45026</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>482188</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>116542</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -679,7 +719,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7278477" cy="3664526"/>
+          <a:ext cx="8173906" cy="3792071"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -734,20 +774,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>638461</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4483</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>307316</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{873124A1-0F4C-91B9-BCCE-0A4F403ABA58}"/>
@@ -769,8 +809,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7924800" y="190500"/>
-          <a:ext cx="4572000" cy="1743075"/>
+          <a:off x="8330179" y="4483"/>
+          <a:ext cx="7360572" cy="2317376"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -782,19 +822,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>8966</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>286871</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>151841</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C5A569E-83A6-2A28-DF8D-4F59E2A18B24}"/>
@@ -816,8 +856,102 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7924800" y="2476500"/>
-          <a:ext cx="4572000" cy="1885950"/>
+          <a:off x="8341660" y="2873188"/>
+          <a:ext cx="7328646" cy="2791947"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C02A4ED-62C8-638A-C8C7-9C725C84393B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{5C5A569E-83A6-2A28-DF8D-4F59E2A18B24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7924800" y="6334125"/>
+          <a:ext cx="4857750" cy="4143375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A9061CD-59B3-F61E-DEB9-F7E8816E945A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4C02A4ED-62C8-638A-C8C7-9C725C84393B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12801600" y="6334125"/>
+          <a:ext cx="4562475" cy="4114800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -831,7 +965,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Brown,AJ" id="{0B403D57-4F86-4C4A-BC48-E244C4E20463}" userId="S::ansleybr@colostate.edu::267c9aa1-a138-42bd-a3c1-9ed3312333cc" providerId="AD"/>
+  <person displayName="Brown,AJ" id="{82DF6874-7F3F-4251-B985-BEFD742A8EAF}" userId="S::ansleybr@colostate.edu::267c9aa1-a138-42bd-a3c1-9ed3312333cc" providerId="AD"/>
 </personList>
 </file>
 
@@ -1098,7 +1232,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A38" dT="2024-07-12T17:36:13.82" personId="{0B403D57-4F86-4C4A-BC48-E244C4E20463}" id="{D0210F6A-9188-4B34-B129-38BBF403A536}">
+  <threadedComment ref="A38" dT="2024-07-12T17:36:13.82" personId="{82DF6874-7F3F-4251-B985-BEFD742A8EAF}" id="{D0210F6A-9188-4B34-B129-38BBF403A536}">
     <text xml:space="preserve">Stewart had a typo submission and it should have been WS25-F2W, so we need to re-submit it below
 </text>
   </threadedComment>
@@ -1107,16 +1241,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E27" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1126,13 +1260,14 @@
     <col min="7" max="7" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="83" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="155.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="11" width="14.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="32.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="83" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="155.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,22 +1298,28 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="10">
+        <v>45489</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1">
         <v>45.909610000000001</v>
@@ -1190,33 +1331,39 @@
         <v>45447</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1">
         <v>46.291578000000001</v>
@@ -1228,33 +1375,39 @@
         <v>45447</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="4">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4">
         <v>45126</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1">
         <v>46.263339999999999</v>
@@ -1266,30 +1419,36 @@
         <v>45447</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1">
         <v>46.252845999999998</v>
@@ -1301,30 +1460,36 @@
         <v>45447</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1">
         <v>46.133496000000001</v>
@@ -1336,30 +1501,36 @@
         <v>45447</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1">
         <v>45.498005999999997</v>
@@ -1371,33 +1542,39 @@
         <v>45449</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="4">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="4">
         <v>45126</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1">
         <v>45.697949000000001</v>
@@ -1409,30 +1586,36 @@
         <v>45449</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1">
         <v>45.898358000000002</v>
@@ -1444,30 +1627,36 @@
         <v>45449</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1">
         <v>45.816850000000002</v>
@@ -1479,33 +1668,39 @@
         <v>45449</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" s="1">
         <v>45.349024</v>
@@ -1517,30 +1712,36 @@
         <v>45468</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="4">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="4">
         <v>45113</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1">
         <v>45.660300999999997</v>
@@ -1552,27 +1753,33 @@
         <v>45468</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="I14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D15" s="1">
         <v>45.431862000000002</v>
@@ -1584,27 +1791,33 @@
         <v>45468</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D16" s="1">
         <v>45.502678000000003</v>
@@ -1616,30 +1829,36 @@
         <v>45468</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>34</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1">
         <v>44.742688000000001</v>
@@ -1651,30 +1870,36 @@
         <v>45469</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>34</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1">
         <v>44.837573999999996</v>
@@ -1686,30 +1911,36 @@
         <v>45469</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1">
         <v>44.837573999999996</v>
@@ -1721,30 +1952,36 @@
         <v>45469</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D22" s="1">
         <v>44.205145999999999</v>
@@ -1756,30 +1993,36 @@
         <v>45470</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>34</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D23" s="1">
         <v>40.542369999999998</v>
@@ -1791,30 +2034,36 @@
         <v>45470</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>34</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D24" s="1">
         <v>41.062220000000003</v>
@@ -1826,30 +2075,36 @@
         <v>45470</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D25" s="1">
         <v>40.774619999999999</v>
@@ -1861,27 +2116,33 @@
         <v>45470</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D26" s="1">
         <v>41.105719999999998</v>
@@ -1893,30 +2154,36 @@
         <v>45470</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>105</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D27" s="1">
         <v>40.581780000000002</v>
@@ -1928,27 +2195,33 @@
         <v>45470</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D29" s="1">
         <v>40.316295459999999</v>
@@ -1960,30 +2233,36 @@
         <v>45474</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D30" s="1">
         <v>44.695286350000003</v>
@@ -1995,27 +2274,33 @@
         <v>45474</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D31" s="1">
         <v>40.144148600000001</v>
@@ -2027,27 +2312,33 @@
         <v>45474</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D32" s="1">
         <v>40.290162100000003</v>
@@ -2059,30 +2350,36 @@
         <v>45474</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="6" t="s">
-        <v>140</v>
+        <v>18</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D33" s="1">
         <v>39.962213920000003</v>
@@ -2094,27 +2391,33 @@
         <v>45474</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M33" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D34" s="1">
         <v>44.5044781</v>
@@ -2126,27 +2429,33 @@
         <v>45474</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D35" s="1">
         <v>40.135103569999998</v>
@@ -2158,30 +2467,36 @@
         <v>45474</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>99</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D37" s="1">
         <v>40.307834999999997</v>
@@ -2193,27 +2508,33 @@
         <v>45482</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="6" t="s">
-        <v>140</v>
+        <v>18</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D38" s="1">
         <v>39.962213920000003</v>
@@ -2225,27 +2546,30 @@
         <v>45482</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D39" s="1">
         <v>40.498097999999999</v>
@@ -2257,36 +2581,41 @@
         <v>45482</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="15"/>
-    <row r="41" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A41" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:12" ht="15">
-      <c r="A43" s="6" t="s">
-        <v>140</v>
+        <v>18</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A41" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:14">
+      <c r="A43" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="D43" s="1">
         <v>39.962214000000003</v>
@@ -2298,15 +2627,15 @@
         <v>45485</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="15">
-      <c r="A44" s="6" t="s">
-        <v>163</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="D44" s="1">
         <v>40.088831999999996</v>
@@ -2318,15 +2647,15 @@
         <v>45485</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D45" s="1">
         <v>40.290692</v>
@@ -2338,15 +2667,15 @@
         <v>45485</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D46" s="1">
         <v>40.790072000000002</v>
@@ -2358,10 +2687,10 @@
         <v>45485</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2378,29 +2707,29 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2410,17 +2739,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1ABFC8-7B09-4026-8E76-8C6972CAAD7A}">
-  <dimension ref="N24"/>
+  <dimension ref="N14:N60"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="24" spans="14:14">
-      <c r="N24" t="s">
-        <v>49</v>
+    <row r="14" spans="14:14">
+      <c r="N14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="14:14">
+      <c r="N32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="14:14">
+      <c r="N60" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2430,15 +2769,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678F2DA36292A241BB6B602A04ACAAD9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e65193b06eae86f79c3903a4a9f0dcf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="167cb1e9-24b5-43e0-9f5d-14a54474cc90" xmlns:ns3="fbf6f0f6-9634-473c-8838-2f74fc79f714" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03593a2a675d04ffa4dc626c9c15704c" ns2:_="" ns3:_="">
     <xsd:import namespace="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
@@ -2693,6 +3023,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2705,11 +3044,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{359EA105-E29C-47C7-80FA-C62692FBF4A4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF35A85-6513-43C2-A7E0-39DEC234E740}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF35A85-6513-43C2-A7E0-39DEC234E740}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{359EA105-E29C-47C7-80FA-C62692FBF4A4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
updated data and made .exe instructions
</commit_message>
<xml_diff>
--- a/output/Delivered to Xin 2024.xlsx
+++ b/output/Delivered to Xin 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colostate.sharepoint.com/sites/AWQP_Sharepoint/Shared Documents/Water_Quality_Project/Research/PileTemp_Cercospora Systems/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansleybr\Documents\GitHub\Ubidots-Python-API-Client-Test\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="384" documentId="13_ncr:1_{A6DA6130-5937-498A-AA95-F2F0CDEC3E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{975090C0-EC95-4706-922E-B4DC02CEC9EA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258290E9-F64B-4BAD-9436-37803B4DB48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="186">
   <si>
     <t>name</t>
   </si>
@@ -588,16 +588,49 @@
   </si>
   <si>
     <t>WS5 showing up as green on dashboard but shows "bad data" for last two days (note on 7/15)</t>
+  </si>
+  <si>
+    <t>WS26-5KL</t>
+  </si>
+  <si>
+    <t>Drab-nb-rt-16</t>
+  </si>
+  <si>
+    <t>Drab-nb-rt-15</t>
+  </si>
+  <si>
+    <t>65d644066eb306000dee50f9</t>
+  </si>
+  <si>
+    <t>65d644067a7226000bcdb493</t>
+  </si>
+  <si>
+    <t>65c3c37648bb6b000e4e9979</t>
+  </si>
+  <si>
+    <t>65c3c377e858cb000eb4367a</t>
+  </si>
+  <si>
+    <t>65d644ba5ee5f8000c3ec157</t>
+  </si>
+  <si>
+    <t>65d644bb7a7226000c15eb7f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -659,10 +692,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -928,7 +961,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A9061CD-59B3-F61E-DEB9-F7E8816E945A}"/>
@@ -1241,16 +1274,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
+      <selection pane="bottomRight" activeCell="A42" sqref="A42:E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1267,7 +1300,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1331,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10">
+      <c r="K1" s="9">
         <v>45489</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1311,7 +1344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1355,7 +1388,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1399,7 +1432,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1440,7 +1473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1481,7 +1514,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1522,7 +1555,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1566,7 +1599,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -1607,7 +1640,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -1648,7 +1681,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -1689,10 +1722,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -1733,7 +1766,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -1771,7 +1804,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1809,7 +1842,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
@@ -1850,7 +1883,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -1891,7 +1924,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -1932,7 +1965,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
@@ -1973,7 +2006,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>89</v>
       </c>
@@ -2014,7 +2047,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>95</v>
       </c>
@@ -2055,7 +2088,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>102</v>
       </c>
@@ -2096,7 +2129,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
@@ -2134,7 +2167,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>112</v>
       </c>
@@ -2175,7 +2208,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>118</v>
       </c>
@@ -2213,7 +2246,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>122</v>
       </c>
@@ -2254,7 +2287,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>127</v>
       </c>
@@ -2292,7 +2325,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>133</v>
       </c>
@@ -2330,7 +2363,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>138</v>
       </c>
@@ -2371,7 +2404,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>144</v>
       </c>
@@ -2409,7 +2442,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>148</v>
       </c>
@@ -2447,7 +2480,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>151</v>
       </c>
@@ -2488,7 +2521,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>156</v>
       </c>
@@ -2526,7 +2559,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>144</v>
       </c>
@@ -2561,7 +2594,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>164</v>
       </c>
@@ -2599,24 +2632,46 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="14.25" customHeight="1">
-      <c r="A41" s="9" t="s">
+    <row r="41" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:14" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:14">
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>144</v>
       </c>
+      <c r="B43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" t="s">
+        <v>146</v>
+      </c>
       <c r="D43" s="1">
         <v>39.962214000000003</v>
       </c>
@@ -2624,7 +2679,7 @@
         <v>-102.29798</v>
       </c>
       <c r="F43" s="2">
-        <v>45485</v>
+        <v>45492</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>125</v>
@@ -2633,10 +2688,16 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>169</v>
       </c>
+      <c r="B44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C44" t="s">
+        <v>181</v>
+      </c>
       <c r="D44" s="1">
         <v>40.088831999999996</v>
       </c>
@@ -2644,7 +2705,7 @@
         <v>-104.418673</v>
       </c>
       <c r="F44" s="2">
-        <v>45485</v>
+        <v>45492</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>125</v>
@@ -2653,10 +2714,16 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>170</v>
       </c>
+      <c r="B45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" t="s">
+        <v>183</v>
+      </c>
       <c r="D45" s="1">
         <v>40.290692</v>
       </c>
@@ -2664,7 +2731,7 @@
         <v>-104.52356399999999</v>
       </c>
       <c r="F45" s="2">
-        <v>45485</v>
+        <v>45492</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>159</v>
@@ -2673,10 +2740,16 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="B46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" t="s">
+        <v>140</v>
+      </c>
       <c r="D46" s="1">
         <v>40.790072000000002</v>
       </c>
@@ -2684,19 +2757,98 @@
         <v>-105.07243099999999</v>
       </c>
       <c r="F46" s="2">
-        <v>45485</v>
+        <v>45492</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>141</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B47" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" s="1">
+        <v>40.130597000000002</v>
+      </c>
+      <c r="E47" s="1">
+        <v>-105.031846</v>
+      </c>
+      <c r="F47" s="2">
+        <v>45492</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D48" s="1">
+        <v>44.896858999999999</v>
+      </c>
+      <c r="E48" s="1">
+        <v>-108.561176</v>
+      </c>
+      <c r="F48" s="2">
+        <v>45492</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" s="1">
+        <v>44.204608999999998</v>
+      </c>
+      <c r="E49" s="1">
+        <v>-107.92478300000001</v>
+      </c>
+      <c r="F49" s="2">
+        <v>45492</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A41:I41"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -2710,24 +2862,24 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -2745,19 +2897,19 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="14" spans="14:14">
+    <row r="14" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="14:14">
+    <row r="32" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="14:14">
+    <row r="60" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N60" t="s">
         <v>176</v>
       </c>
@@ -2769,6 +2921,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678F2DA36292A241BB6B602A04ACAAD9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e65193b06eae86f79c3903a4a9f0dcf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="167cb1e9-24b5-43e0-9f5d-14a54474cc90" xmlns:ns3="fbf6f0f6-9634-473c-8838-2f74fc79f714" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03593a2a675d04ffa4dc626c9c15704c" ns2:_="" ns3:_="">
     <xsd:import namespace="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
@@ -3023,34 +3195,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF35A85-6513-43C2-A7E0-39DEC234E740}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{013FE671-D777-4E39-B7A9-097643CB5B67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
+    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{359EA105-E29C-47C7-80FA-C62692FBF4A4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{359EA105-E29C-47C7-80FA-C62692FBF4A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{013FE671-D777-4E39-B7A9-097643CB5B67}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF35A85-6513-43C2-A7E0-39DEC234E740}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
+    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>